<commit_message>
Changed logic for ReadObject
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6174D8D1-2AD3-4869-A092-3F2FE6BAB60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CA5984-94C9-406E-8420-CB1EA937909E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="80">
   <si>
     <t>TestCase</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Quickorder_SCROLL</t>
+  </si>
+  <si>
+    <t>Xpath</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -947,7 +950,7 @@
         <v>62</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="E18" s="7"/>
     </row>

</xml_diff>

<commit_message>
Enabling TC03 for ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D09C78-568D-4CAA-883B-E6FB82E225CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E5109D-9D0D-4CE3-9D4B-8DCC9A2CE27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC40_Adding_MultipleItems_Quick" sheetId="1" r:id="rId1"/>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1956,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2221,15 +2221,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100599AB90ED4ADBD46B68D7A0832AE2D34" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d93929aa8d4e603f371af1ff5e0b517">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6243fcc-5e87-4459-985d-7491a55b4be2" xmlns:ns3="904b644c-3cf7-40e5-b5a5-e101a1ff52b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17e9716027504630c423500e26042861" ns2:_="" ns3:_="">
     <xsd:import namespace="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
@@ -2440,6 +2431,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2447,14 +2447,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAE325E-5F3B-4FE5-B026-F899F4FA3755}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2469,6 +2461,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>